<commit_message>
merged with spark jobs for embeddings
</commit_message>
<xml_diff>
--- a/text_rec_results.xlsx
+++ b/text_rec_results.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.renner\TextRecResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\j.renner\TextRecResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA7DB1E-19D2-435E-809C-F020C6D26530}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>Method</t>
   </si>
@@ -51,13 +52,25 @@
   </si>
   <si>
     <t>Window Size</t>
+  </si>
+  <si>
+    <t>ProdWord2Vec</t>
+  </si>
+  <si>
+    <t>Word Weighting</t>
+  </si>
+  <si>
+    <t>tfidf</t>
+  </si>
+  <si>
+    <t>uniform</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +82,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,9 +116,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -412,16 +435,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,80 +454,83 @@
       <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
         <v>25</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>1.00038476337052E-3</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>5.6671033625361397E-3</v>
       </c>
-      <c r="F2" s="1">
-        <v>8.8495575221238904E-4</v>
-      </c>
       <c r="G2" s="1">
-        <v>4.8424309067302404E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+        <v>1.00038476337052E-3</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5.6671033625361397E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
         <v>50</v>
       </c>
-      <c r="D3">
-        <v>1.5390534821084999E-3</v>
-      </c>
       <c r="E3">
-        <v>8.4337994602136802E-3</v>
+        <v>1.59676798768756E-3</v>
       </c>
       <c r="F3">
-        <v>1.0388611004232299E-3</v>
-      </c>
-      <c r="G3">
-        <v>5.1335057839555203E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8.8026570135895394E-3</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.5582916506348501E-3</v>
+      </c>
+      <c r="H3" s="2">
+        <v>8.6785184961932493E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
         <v>100</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1.3466717968449299E-3</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>8.2923226745443002E-3</v>
       </c>
-      <c r="F4">
-        <v>1.11581377452866E-3</v>
-      </c>
       <c r="G4">
-        <v>6.2268163539161503E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+        <v>1.3466717968449299E-3</v>
+      </c>
+      <c r="H4">
+        <v>8.2923226745443002E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -514,20 +540,20 @@
       <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1.07541362062332E-2</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>4.9252926981654101E-2</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1.07733743747595E-3</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>5.8850580428803896E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -537,20 +563,20 @@
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="E6" s="3">
         <v>1.26394767218161E-2</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>6.0849386077138197E-2</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>8.0800307810696399E-4</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>4.3796206328408803E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -560,8 +586,20 @@
       <c r="C7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E7">
+        <v>1.2524047710657999E-2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>6.5447976587353504E-2</v>
+      </c>
+      <c r="G7">
+        <v>8.65717583686033E-4</v>
+      </c>
+      <c r="H7">
+        <v>4.7150872562152996E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -571,8 +609,20 @@
       <c r="C8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E8">
+        <v>9.8114659484417905E-3</v>
+      </c>
+      <c r="F8">
+        <v>4.6397192349962403E-2</v>
+      </c>
+      <c r="G8">
+        <v>6.9257406694882599E-4</v>
+      </c>
+      <c r="H8">
+        <v>4.6865417366717304E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -582,8 +632,20 @@
       <c r="C9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E9" s="2">
+        <v>1.4024624855713701E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>6.7112001487567199E-2</v>
+      </c>
+      <c r="G9">
+        <v>1.11581377452866E-3</v>
+      </c>
+      <c r="H9">
+        <v>5.6959708234617301E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -593,14 +655,165 @@
       <c r="C10">
         <v>3</v>
       </c>
+      <c r="E10">
+        <v>1.3639861485186601E-2</v>
+      </c>
+      <c r="F10">
+        <v>6.3758922736521395E-2</v>
+      </c>
+      <c r="G10">
+        <v>8.48133863686033E-4</v>
+      </c>
+      <c r="H10">
+        <v>4.7079185862153004E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11">
+        <v>8.46479415159683E-3</v>
+      </c>
+      <c r="F11">
+        <v>4.8245424301151703E-2</v>
+      </c>
+      <c r="G11">
+        <v>2.3470565602154601E-3</v>
+      </c>
+      <c r="H11">
+        <v>1.1803630366097001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>8.3493651404386894E-3</v>
+      </c>
+      <c r="F12">
+        <v>5.0031575072219003E-2</v>
+      </c>
+      <c r="G12">
+        <v>2.7125817622162302E-3</v>
+      </c>
+      <c r="H12">
+        <v>1.36490289779198E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>200</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>7.7145055790689299E-3</v>
+      </c>
+      <c r="F13">
+        <v>4.5540062899378703E-2</v>
+      </c>
+      <c r="G13">
+        <v>2.8664871104270798E-3</v>
+      </c>
+      <c r="H13">
+        <v>1.3932971840025499E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>9.6383224317045796E-3</v>
+      </c>
+      <c r="F14">
+        <v>5.4303058820772E-2</v>
+      </c>
+      <c r="G14">
+        <v>2.6741054251635098E-3</v>
+      </c>
+      <c r="H14">
+        <v>1.23542901107217E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2">
+        <v>9.5806079261255093E-3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>5.4419743212762203E-2</v>
+      </c>
+      <c r="G15" s="2">
+        <v>3.3089649865332702E-3</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.6322618366025901E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>200</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>9.7537514428627202E-3</v>
+      </c>
+      <c r="F16">
+        <v>5.4268502405740902E-2</v>
+      </c>
+      <c r="G16">
+        <v>3.1550596383224201E-3</v>
+      </c>
+      <c r="H16">
+        <v>1.6580330222818799E-2</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1"/>
-    <hyperlink ref="E1" r:id="rId2"/>
-    <hyperlink ref="F1" r:id="rId3"/>
-    <hyperlink ref="G1" r:id="rId4"/>
+    <hyperlink ref="E1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F1" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G1" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H1" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>